<commit_message>
highlights removed from riskdrivers excel
</commit_message>
<xml_diff>
--- a/Data/Risk_drivers.xlsx
+++ b/Data/Risk_drivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D620C70-DB58-44BE-855D-24DD0E74FA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAF2BDF-645D-4E07-9BA3-F99BEDAEEE7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
+    <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -624,18 +624,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -667,7 +661,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -987,7 +981,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -1695,23 +1689,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012622E045E3264E917E2E70247D59DA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="790fdbb8542707c675f15d468791c78c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="95ec377a-6541-4b84-af39-d48b8b06c521" xmlns:ns4="5f881008-17d2-4d16-90e0-937d4120d730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d3917910e9e8daf493e8495c95b1d7d" ns3:_="" ns4:_="">
     <xsd:import namespace="95ec377a-6541-4b84-af39-d48b8b06c521"/>
@@ -1894,32 +1871,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B582907-3412-4C04-9444-C284B34F4904}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1936,4 +1905,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
change example text risk driver 2.2
</commit_message>
<xml_diff>
--- a/Data/Risk_drivers.xlsx
+++ b/Data/Risk_drivers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46B3782C-269E-4C09-8E4E-25A70B76BD92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5070FF4-B0AD-4F59-9757-7FB209D9FFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
@@ -536,15 +536,6 @@
     <t>Medium diverse Management Team on certain (but not all) aspects of diversity on e.g. Ethnical background, Gender, Type of working experience (e.g. start-up, scale-up, corporate, institution) and Personality types (green/red/yellow/blue)</t>
   </si>
   <si>
-    <t>No incentives for efficient use of product (e.g. rental contract with fixed fee)</t>
-  </si>
-  <si>
-    <t>Some incentives for efficient use of product</t>
-  </si>
-  <si>
-    <t>Pay-per-use/sharing model: efficient use of product by users. Less products needed overall (e.g. wash-as-a-service)</t>
-  </si>
-  <si>
     <t>Relatively fast peak extraction year (&lt; 2031)</t>
   </si>
   <si>
@@ -588,6 +579,15 @@
   </si>
   <si>
     <t>3.1 Dependency on critical raw materials (Please refer to the tab sheet 'Peak extraction years' to match the key materials used in the product with peak extraction years)</t>
+  </si>
+  <si>
+    <t>Partly performance based contract, including at least one incentive for efficient use of product (e.g. fee differentiation between sustainable vs unsustainable use (e.g. Homie: discount for short wash at lower temperature), incentive to perform maintenance (e.g. incentive to perform a maintenenace wash) and/or discount for returned goods in a good condition).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pay-per-use/sharing model: efficient use of product by multiple users (e.g. pay-per-wash), with as a result less products needed overall. </t>
+  </si>
+  <si>
+    <t>No incentives for efficient use of product (e.g. rental contract with fixed fee).</t>
   </si>
 </sst>
 </file>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC94184-36DC-4334-8EC3-79CE319DCC44}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1143,15 +1143,15 @@
         <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.35">
       <c r="D14" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1159,7 +1159,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -1170,10 +1170,10 @@
         <v>88</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>113</v>
@@ -1184,7 +1184,7 @@
         <v>163</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>114</v>
@@ -1192,10 +1192,10 @@
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>115</v>
@@ -1206,7 +1206,7 @@
         <v>89</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>116</v>
@@ -1217,7 +1217,7 @@
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>117</v>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D21" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>118</v>
@@ -1233,7 +1233,7 @@
     </row>
     <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="D22" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>119</v>
@@ -1296,7 +1296,7 @@
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>29</v>
@@ -1345,7 +1345,7 @@
     </row>
     <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D33" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>129</v>
@@ -1465,7 +1465,7 @@
         <v>96</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>141</v>
@@ -1500,10 +1500,10 @@
     </row>
     <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D49" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
         <v>61</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1686,23 +1686,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012622E045E3264E917E2E70247D59DA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="790fdbb8542707c675f15d468791c78c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="95ec377a-6541-4b84-af39-d48b8b06c521" xmlns:ns4="5f881008-17d2-4d16-90e0-937d4120d730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d3917910e9e8daf493e8495c95b1d7d" ns3:_="" ns4:_="">
     <xsd:import namespace="95ec377a-6541-4b84-af39-d48b8b06c521"/>
@@ -1885,32 +1868,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B582907-3412-4C04-9444-C284B34F4904}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1927,4 +1902,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed overwrite to override in riskdrivers excel
</commit_message>
<xml_diff>
--- a/Data/Risk_drivers.xlsx
+++ b/Data/Risk_drivers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6947768-484C-4322-9A93-95DBCB88E7DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69C1512-E04D-46C8-935A-F9D1B7C1E7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
@@ -338,9 +338,6 @@
     <t>Very competitive</t>
   </si>
   <si>
-    <t>Overwrites</t>
-  </si>
-  <si>
     <t>Example</t>
   </si>
   <si>
@@ -588,6 +585,9 @@
   </si>
   <si>
     <t>Suitability for circular proposition</t>
+  </si>
+  <si>
+    <t>Overrides</t>
   </si>
 </sst>
 </file>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC94184-36DC-4334-8EC3-79CE319DCC44}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,7 +996,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>100</v>
+        <v>183</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -1005,7 +1005,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
@@ -1022,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1033,7 +1033,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1044,7 +1044,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1055,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1066,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1074,7 +1074,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1082,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1090,12 +1090,12 @@
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>83</v>
@@ -1107,7 +1107,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1118,7 +1118,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1129,7 +1129,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1143,15 +1143,15 @@
         <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.35">
       <c r="D14" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1159,7 +1159,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -1170,35 +1170,35 @@
         <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1206,10 +1206,10 @@
         <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1217,26 +1217,26 @@
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D21" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="D22" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1247,7 +1247,7 @@
         <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1255,7 +1255,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1263,7 +1263,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1280,7 +1280,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1291,18 +1291,18 @@
         <v>28</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1313,7 +1313,7 @@
         <v>30</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1324,7 +1324,7 @@
         <v>33</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1332,7 +1332,7 @@
         <v>34</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1340,15 +1340,15 @@
         <v>35</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D33" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1359,7 +1359,7 @@
         <v>37</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>38</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1375,7 +1375,7 @@
         <v>39</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1383,7 +1383,7 @@
         <v>40</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1394,7 +1394,7 @@
         <v>42</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1402,7 +1402,7 @@
         <v>43</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1410,7 +1410,7 @@
         <v>44</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1418,7 +1418,7 @@
         <v>45</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>48</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1446,7 +1446,7 @@
         <v>49</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1457,7 +1457,7 @@
         <v>50</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1465,10 +1465,10 @@
         <v>95</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1479,7 +1479,7 @@
         <v>52</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1487,7 +1487,7 @@
         <v>53</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1495,15 +1495,15 @@
         <v>54</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D49" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>177</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1522,7 +1522,7 @@
         <v>57</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1530,7 +1530,7 @@
         <v>58</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1547,7 +1547,7 @@
         <v>63</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1558,7 +1558,7 @@
         <v>62</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
         <v>61</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1583,7 +1583,7 @@
         <v>65</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1591,7 +1591,7 @@
         <v>66</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1599,7 +1599,7 @@
         <v>67</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="48" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
         <v>68</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1618,7 +1618,7 @@
         <v>70</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1626,7 +1626,7 @@
         <v>71</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1634,7 +1634,7 @@
         <v>72</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1642,7 +1642,7 @@
         <v>73</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1653,7 +1653,7 @@
         <v>75</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="4:5" ht="48" x14ac:dyDescent="0.35">
@@ -1661,15 +1661,15 @@
         <v>76</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="4:5" ht="48" x14ac:dyDescent="0.35">
       <c r="D66" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="4:5" ht="36" x14ac:dyDescent="0.35">
@@ -1677,7 +1677,7 @@
         <v>77</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -1686,12 +1686,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1878,17 +1877,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1913,18 +1922,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed answers for riskdriver 1.1
</commit_message>
<xml_diff>
--- a/Data/Risk_drivers.xlsx
+++ b/Data/Risk_drivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B69C1512-E04D-46C8-935A-F9D1B7C1E7A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E60949D7-1876-4451-BBE0-B1E3579D4A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
+    <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -341,18 +341,6 @@
     <t>Example</t>
   </si>
   <si>
-    <t>Management Team has in total &lt;1 years as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
-  </si>
-  <si>
-    <t>Management Team has in total 1-5 years of experience as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
-  </si>
-  <si>
-    <t>Management Team has in total 5-20 years of experience as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
-  </si>
-  <si>
-    <t>Management Team has in total &gt;20 years of experience as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
-  </si>
-  <si>
     <t>No diversity in Management Team on e.g. Ethnical background, Gender, Type of working experience (e.g. start-up, scale-up, corporate, institution) and Personality types (green/red/yellow/blue)</t>
   </si>
   <si>
@@ -588,6 +576,18 @@
   </si>
   <si>
     <t>Overrides</t>
+  </si>
+  <si>
+    <t>Management Team has on average per MT-member &lt;1 years as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
+  </si>
+  <si>
+    <t>Management Team has on average per MT-member 1-5 years of experience as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
+  </si>
+  <si>
+    <t>Management Team has on average per MT-member 5-20 years of experience as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
+  </si>
+  <si>
+    <t>Management Team has on average per MT-member &gt;20 years of experience as a board member/leader/management team of innovative, circular and/or PaaS businesses</t>
   </si>
 </sst>
 </file>
@@ -978,7 +978,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -996,7 +996,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -1022,10 +1022,10 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
         <v>80</v>
       </c>
@@ -1033,10 +1033,10 @@
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>81</v>
       </c>
@@ -1044,10 +1044,10 @@
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>104</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1066,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1074,7 +1074,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1082,7 +1082,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1090,12 +1090,12 @@
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>83</v>
@@ -1107,7 +1107,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1118,7 +1118,7 @@
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1129,7 +1129,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1143,15 +1143,15 @@
         <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.35">
       <c r="D14" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1159,7 +1159,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -1170,35 +1170,35 @@
         <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1206,10 +1206,10 @@
         <v>88</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1217,26 +1217,26 @@
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D21" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="D22" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1247,7 +1247,7 @@
         <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1255,7 +1255,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1263,7 +1263,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1280,7 +1280,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1291,18 +1291,18 @@
         <v>28</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1313,7 +1313,7 @@
         <v>30</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1324,7 +1324,7 @@
         <v>33</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1332,7 +1332,7 @@
         <v>34</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1340,15 +1340,15 @@
         <v>35</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D33" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1359,7 +1359,7 @@
         <v>37</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>38</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1375,7 +1375,7 @@
         <v>39</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1383,7 +1383,7 @@
         <v>40</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1394,7 +1394,7 @@
         <v>42</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1402,7 +1402,7 @@
         <v>43</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1410,7 +1410,7 @@
         <v>44</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1418,7 +1418,7 @@
         <v>45</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>48</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1446,7 +1446,7 @@
         <v>49</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1457,7 +1457,7 @@
         <v>50</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1465,10 +1465,10 @@
         <v>95</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1479,7 +1479,7 @@
         <v>52</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1487,7 +1487,7 @@
         <v>53</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1495,15 +1495,15 @@
         <v>54</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D49" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1522,7 +1522,7 @@
         <v>57</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1530,7 +1530,7 @@
         <v>58</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1547,7 +1547,7 @@
         <v>63</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1558,7 +1558,7 @@
         <v>62</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1569,7 +1569,7 @@
         <v>61</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1583,7 +1583,7 @@
         <v>65</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1591,7 +1591,7 @@
         <v>66</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1599,7 +1599,7 @@
         <v>67</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="48" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
         <v>68</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1618,7 +1618,7 @@
         <v>70</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1626,7 +1626,7 @@
         <v>71</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1634,7 +1634,7 @@
         <v>72</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1642,7 +1642,7 @@
         <v>73</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1653,7 +1653,7 @@
         <v>75</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="4:5" ht="48" x14ac:dyDescent="0.35">
@@ -1661,15 +1661,15 @@
         <v>76</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="66" spans="4:5" ht="48" x14ac:dyDescent="0.35">
       <c r="D66" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="67" spans="4:5" ht="36" x14ac:dyDescent="0.35">
@@ -1677,7 +1677,7 @@
         <v>77</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1686,11 +1686,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1877,27 +1878,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1922,9 +1913,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{937E51E9-E945-4071-9915-DFEA9D97EED8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to 4.1, one less answer option
</commit_message>
<xml_diff>
--- a/Data/Risk_drivers.xlsx
+++ b/Data/Risk_drivers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F6CBD6-58E4-40A7-960D-F8A0454C989A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647C2D54-A19C-4E64-97E0-489E8E08E2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <si>
     <t>1.1 Experience Management Team with innovative / circular businesses</t>
   </si>
@@ -119,12 +119,6 @@
     <t>Circularity of asset</t>
   </si>
   <si>
-    <t>Not modular and not able to upgrade</t>
-  </si>
-  <si>
-    <t>Not modular, hard to upgrade</t>
-  </si>
-  <si>
     <t>Partly modular, not so easy to upgrade</t>
   </si>
   <si>
@@ -368,12 +362,6 @@
     <t>Strong cooperation with suppliers, e.g. one or more projects in which supplier and business invest together or share a common name</t>
   </si>
   <si>
-    <t>Product and parts cannot be upgraded</t>
-  </si>
-  <si>
-    <t>Product is very difficult to change or upgrade</t>
-  </si>
-  <si>
     <t>Some parts of the product can be changed or adapted to changing market standards</t>
   </si>
   <si>
@@ -591,6 +579,12 @@
   </si>
   <si>
     <t>Share of company 10-25% of total circular market</t>
+  </si>
+  <si>
+    <t>Product is very difficult to change or upgrade, or cannot be upgraded at all</t>
+  </si>
+  <si>
+    <t>Not modular, and very hard to upgrade</t>
   </si>
 </sst>
 </file>
@@ -978,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC94184-36DC-4334-8EC3-79CE319DCC44}">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -999,7 +993,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -1008,15 +1002,15 @@
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1025,40 +1019,40 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1069,7 +1063,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1077,7 +1071,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1085,7 +1079,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1093,15 +1087,15 @@
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>13</v>
@@ -1110,34 +1104,34 @@
         <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
@@ -1146,15 +1140,15 @@
         <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.35">
       <c r="D14" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1162,7 +1156,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -1170,49 +1164,49 @@
         <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1220,26 +1214,26 @@
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D21" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="D22" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1250,7 +1244,7 @@
         <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1258,7 +1252,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1266,7 +1260,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1274,413 +1268,405 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="B27" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B27" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="E27" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C30" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="D30" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E30" s="4" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D32" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="C33" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E33" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="D34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D35" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="D33" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="C34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="D35" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D36" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C37" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D37" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="E38" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D39" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D40" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="B41" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B42" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D41" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E41" s="4" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" s="1" t="s">
+    <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="D45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B44" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="4" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B45" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C46" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="D48" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="C49" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="D48" s="1" t="s">
+      <c r="D49" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="D49" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="C50" s="2" t="s">
-        <v>55</v>
-      </c>
+    </row>
+    <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D50" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>56</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D51" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="D52" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="B53" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C53" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D53" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="E53" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="B55" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D54" s="1" t="s">
+      <c r="C55" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="D55" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B55" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>159</v>
-      </c>
-    </row>
     <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="B56" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D56" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="E56" s="4" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D57" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="48" x14ac:dyDescent="0.35">
+      <c r="D58" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="D58" s="1" t="s">
+      <c r="E58" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="C59" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E58" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="48" x14ac:dyDescent="0.35">
-      <c r="D59" s="1" t="s">
-        <v>66</v>
+      <c r="D59" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="C60" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D60" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D61" s="4" t="s">
-        <v>184</v>
+        <v>66</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D62" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="C63" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E62" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="D63" s="4" t="s">
+      <c r="D63" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="C64" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="48" x14ac:dyDescent="0.35">
+      <c r="D64" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="E64" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="4:5" ht="48" x14ac:dyDescent="0.35">
       <c r="D65" s="1" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="66" spans="4:5" ht="48" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="4:5" ht="36" x14ac:dyDescent="0.35">
       <c r="D66" s="1" t="s">
-        <v>149</v>
+        <v>71</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="67" spans="4:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="D67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1689,23 +1675,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012622E045E3264E917E2E70247D59DA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="790fdbb8542707c675f15d468791c78c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="95ec377a-6541-4b84-af39-d48b8b06c521" xmlns:ns4="5f881008-17d2-4d16-90e0-937d4120d730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d3917910e9e8daf493e8495c95b1d7d" ns3:_="" ns4:_="">
     <xsd:import namespace="95ec377a-6541-4b84-af39-d48b8b06c521"/>
@@ -1888,10 +1857,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B582907-3412-4C04-9444-C284B34F4904}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
+    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1914,20 +1911,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B582907-3412-4C04-9444-C284B34F4904}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
-    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes to 6.2, one less answer option
</commit_message>
<xml_diff>
--- a/Data/Risk_drivers.xlsx
+++ b/Data/Risk_drivers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{647C2D54-A19C-4E64-97E0-489E8E08E2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD9574C-0EDA-4AB5-90C9-830AEF6A512F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-10760" windowWidth="38620" windowHeight="21220" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t>1.1 Experience Management Team with innovative / circular businesses</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Some circular and/or existing linear competitors</t>
   </si>
   <si>
-    <t>Niche circular market, no linear alternative available</t>
-  </si>
-  <si>
     <t>6.3 Circular marketshare</t>
   </si>
   <si>
@@ -429,9 +426,6 @@
   </si>
   <si>
     <t>Medium upfront investments needed, medium-tech products</t>
-  </si>
-  <si>
-    <t>No (real) examples as of yet. But, for example, an innovation that requires no material / appliance to wash clothes, e.g. clothing that needs no washing. Would be new circular product (given the clothing material itself is circular, without a linear alternative).</t>
   </si>
   <si>
     <t xml:space="preserve">E.g. circular artificial flowers, not many circular competitors, but not many linear artificial flower suppliers either </t>
@@ -972,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC94184-36DC-4334-8EC3-79CE319DCC44}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -993,7 +987,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -1002,15 +996,15 @@
         <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -1019,40 +1013,40 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1063,7 +1057,7 @@
         <v>6</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1071,7 +1065,7 @@
         <v>7</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1079,7 +1073,7 @@
         <v>8</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.35">
@@ -1087,15 +1081,15 @@
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>13</v>
@@ -1104,34 +1098,34 @@
         <v>14</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>19</v>
@@ -1140,15 +1134,15 @@
         <v>17</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.35">
       <c r="D14" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1156,7 +1150,7 @@
         <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="87" x14ac:dyDescent="0.35">
@@ -1164,49 +1158,49 @@
         <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1214,26 +1208,26 @@
         <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D21" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="D22" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1244,7 +1238,7 @@
         <v>23</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1252,7 +1246,7 @@
         <v>24</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1260,7 +1254,7 @@
         <v>25</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1268,43 +1262,43 @@
         <v>26</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B27" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B29" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>30</v>
@@ -1313,7 +1307,7 @@
         <v>31</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1321,7 +1315,7 @@
         <v>32</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1329,15 +1323,15 @@
         <v>33</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D32" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1348,7 +1342,7 @@
         <v>35</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1356,7 +1350,7 @@
         <v>36</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1364,7 +1358,7 @@
         <v>37</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1372,7 +1366,7 @@
         <v>38</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1383,7 +1377,7 @@
         <v>40</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1391,7 +1385,7 @@
         <v>41</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1399,7 +1393,7 @@
         <v>42</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1407,7 +1401,7 @@
         <v>43</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1415,7 +1409,7 @@
         <v>44</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>45</v>
@@ -1424,40 +1418,40 @@
         <v>46</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>48</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1468,7 +1462,7 @@
         <v>50</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -1476,7 +1470,7 @@
         <v>51</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1484,15 +1478,15 @@
         <v>52</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D48" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1500,7 +1494,7 @@
         <v>53</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>54</v>
@@ -1508,18 +1502,18 @@
     </row>
     <row r="50" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D50" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D51" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="29" x14ac:dyDescent="0.35">
@@ -1527,7 +1521,7 @@
         <v>55</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>56</v>
@@ -1536,34 +1530,34 @@
         <v>59</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>60</v>
@@ -1572,7 +1566,7 @@
         <v>61</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1580,7 +1574,7 @@
         <v>62</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1588,34 +1582,34 @@
         <v>63</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="48" x14ac:dyDescent="0.35">
-      <c r="D58" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="24" x14ac:dyDescent="0.35">
+      <c r="C58" s="2" t="s">
         <v>64</v>
       </c>
+      <c r="D58" s="4" t="s">
+        <v>177</v>
+      </c>
       <c r="E58" s="4" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="C59" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="D59" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="24" x14ac:dyDescent="0.35">
       <c r="D60" s="4" t="s">
-        <v>180</v>
+        <v>65</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="24" x14ac:dyDescent="0.35">
@@ -1623,50 +1617,42 @@
         <v>66</v>
       </c>
       <c r="E61" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="C62" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="24" x14ac:dyDescent="0.35">
-      <c r="D62" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="C63" s="2" t="s">
-        <v>68</v>
-      </c>
+    <row r="63" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="D63" s="1" t="s">
         <v>69</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="48" x14ac:dyDescent="0.35">
       <c r="D64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="D65" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E64" s="4" t="s">
+      <c r="E65" s="4" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="65" spans="4:5" ht="48" x14ac:dyDescent="0.35">
-      <c r="D65" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="66" spans="4:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="D66" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1675,6 +1661,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100012622E045E3264E917E2E70247D59DA" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="790fdbb8542707c675f15d468791c78c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="95ec377a-6541-4b84-af39-d48b8b06c521" xmlns:ns4="5f881008-17d2-4d16-90e0-937d4120d730" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d3917910e9e8daf493e8495c95b1d7d" ns3:_="" ns4:_="">
     <xsd:import namespace="95ec377a-6541-4b84-af39-d48b8b06c521"/>
@@ -1857,38 +1860,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="95ec377a-6541-4b84-af39-d48b8b06c521" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B582907-3412-4C04-9444-C284B34F4904}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
-    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1911,9 +1886,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D203786-B4DC-419B-960A-C4C5F2896F74}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B582907-3412-4C04-9444-C284B34F4904}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="95ec377a-6541-4b84-af39-d48b8b06c521"/>
+    <ds:schemaRef ds:uri="5f881008-17d2-4d16-90e0-937d4120d730"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
minor update (changes suggested by Jeroen and Manon)
</commit_message>
<xml_diff>
--- a/Data/Risk_drivers.xlsx
+++ b/Data/Risk_drivers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\Repo\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DiederikHemmesRiskQu\Documents\Circular Finance\dashboard\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17E8624-A87C-4D9B-B5BF-AE300E0CEA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352E860D-7F14-465E-898A-D286D4B042C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-10930" windowWidth="38620" windowHeight="21220" xr2:uid="{3D4E5762-CCCC-4F58-8FC2-83722782063A}"/>
   </bookViews>
@@ -404,12 +404,6 @@
     <t>Closed loop, company remains ownership of assets (pay per use, buy-back guarantee)</t>
   </si>
   <si>
-    <t>&gt; 10 years</t>
-  </si>
-  <si>
-    <t>&gt;75% non-virgin / bio-based materials</t>
-  </si>
-  <si>
     <t>High upfront investments needed (e.g. industry), high-tech products</t>
   </si>
   <si>
@@ -601,6 +595,12 @@
   </si>
   <si>
     <t>Company is regarded as sustainable frontrunner in both current and future policies</t>
+  </si>
+  <si>
+    <t>\&gt;75% non-virgin / bio-based materials</t>
+  </si>
+  <si>
+    <t>\&gt; 10 years</t>
   </si>
 </sst>
 </file>
@@ -690,7 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -716,112 +716,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1156,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC94184-36DC-4334-8EC3-79CE319DCC44}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52:E65"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1181,7 +1079,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>11</v>
@@ -1193,29 +1091,29 @@
         <v>73</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1224,8 +1122,8 @@
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>130</v>
+      <c r="E2" s="4" t="s">
+        <v>128</v>
       </c>
       <c r="F2" s="6">
         <v>1</v>
@@ -1247,46 +1145,46 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="4" t="s">
         <v>60</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>131</v>
+      <c r="E3" s="9" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="B4" s="10" t="s">
-        <v>146</v>
+      <c r="B4" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>148</v>
+      <c r="E4" s="9" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="B5" s="10" t="s">
-        <v>147</v>
+      <c r="B5" s="9" t="s">
+        <v>145</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>149</v>
+      <c r="E5" s="9" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="F6" s="6">
@@ -1309,101 +1207,101 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
+      <c r="C7"/>
+      <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
+      <c r="C8"/>
+      <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="C9" s="13"/>
-      <c r="D9" s="14" t="s">
+      <c r="C9"/>
+      <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="4" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="F10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="48" x14ac:dyDescent="0.35">
+      <c r="B11" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E11" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="F10" s="6">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="48" x14ac:dyDescent="0.35">
-      <c r="B11" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="19" t="s">
+    </row>
+    <row r="12" spans="1:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="D12" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E12" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="B12" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="19" t="s">
+    <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="B13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>157</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="B13" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>159</v>
       </c>
       <c r="F13" s="7">
         <v>0</v>
@@ -1425,21 +1323,21 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="60" x14ac:dyDescent="0.35">
-      <c r="C14" s="21"/>
-      <c r="D14" s="22" t="s">
+      <c r="C14"/>
+      <c r="D14" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="E14" s="22" t="s">
-        <v>160</v>
+      <c r="E14" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="C15" s="21"/>
-      <c r="D15" s="22" t="s">
+      <c r="C15"/>
+      <c r="D15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="22" t="s">
-        <v>161</v>
+      <c r="E15" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="84" x14ac:dyDescent="0.35">
@@ -1449,14 +1347,14 @@
       <c r="B16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>162</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>164</v>
       </c>
       <c r="F16" s="6">
         <v>1</v>
@@ -1481,43 +1379,43 @@
       <c r="B17" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>166</v>
+      <c r="D17" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="84" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>168</v>
+        <v>123</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="48" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>170</v>
+      <c r="D19" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="E20" s="26" t="s">
+      <c r="E20" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F20" s="6">
@@ -1540,63 +1438,63 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E22" s="26" t="s">
-        <v>132</v>
+      <c r="E22" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="C23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="27" t="s">
+      <c r="D23" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>1</v>
+      </c>
+      <c r="I23" s="2">
+        <v>1</v>
+      </c>
+      <c r="J23" s="2">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="D24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="D25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E23" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2">
-        <v>1</v>
-      </c>
-      <c r="H23" s="2">
-        <v>1</v>
-      </c>
-      <c r="I23" s="2">
-        <v>1</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1</v>
-      </c>
-      <c r="K23" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="D24" s="27" t="s">
-        <v>172</v>
-      </c>
-      <c r="E24" s="28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="D25" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="4" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1604,17 +1502,17 @@
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="E26" s="30" t="s">
-        <v>138</v>
+      <c r="D26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>136</v>
       </c>
       <c r="F26" s="7">
         <v>0</v>
@@ -1636,29 +1534,29 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="B27" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="D27" s="29" t="s">
+      <c r="B27" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="4" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="B28" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="D28" s="29" t="s">
+      <c r="B28" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="29" x14ac:dyDescent="0.35">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1707,7 +1605,7 @@
     </row>
     <row r="32" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="D32" s="1" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>86</v>
@@ -1717,10 +1615,10 @@
       <c r="C33" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="4" t="s">
         <v>87</v>
       </c>
       <c r="F33" s="8">
@@ -1743,26 +1641,26 @@
       </c>
     </row>
     <row r="34" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E35" s="35" t="s">
+      <c r="E35" s="4" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="35" t="s">
+      <c r="E36" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1770,10 +1668,10 @@
       <c r="C37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="36" t="s">
+      <c r="D37" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="36" t="s">
+      <c r="E37" s="4" t="s">
         <v>91</v>
       </c>
       <c r="F37" s="7">
@@ -1796,26 +1694,26 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D38" s="36" t="s">
+      <c r="D38" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="4" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D39" s="36" t="s">
+      <c r="D39" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E39" s="36" t="s">
+      <c r="E39" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="D40" s="36" t="s">
+      <c r="D40" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="36" t="s">
+      <c r="E40" s="4" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1823,13 +1721,13 @@
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="33" t="s">
+      <c r="B41" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D41" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E41" s="4" t="s">
@@ -1855,10 +1753,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="D42" s="4" t="s">
         <v>40</v>
       </c>
       <c r="E42" s="4" t="s">
@@ -1866,10 +1764,10 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B43" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="B43" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E43" s="4" t="s">
@@ -1877,11 +1775,11 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>122</v>
+      <c r="D44" s="4" t="s">
+        <v>186</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>98</v>
@@ -1934,20 +1832,20 @@
     </row>
     <row r="48" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="D48" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="C49" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="D49" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="E49" s="38" t="s">
+      <c r="C49" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F49" s="7">
@@ -1970,35 +1868,35 @@
       </c>
     </row>
     <row r="50" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="D50" s="39" t="s">
+      <c r="D50" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="D51" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E51" s="9" t="s">
         <v>177</v>
-      </c>
-      <c r="E50" s="39" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="D51" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="E51" s="39" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="24" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="40" t="s">
+      <c r="B52" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C52" s="44" t="s">
+      <c r="C52" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="43" t="s">
+      <c r="D52" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E52" s="44" t="s">
+      <c r="E52" s="4" t="s">
         <v>103</v>
       </c>
       <c r="F52" s="6">
@@ -2021,187 +1919,187 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B53" s="40" t="s">
+      <c r="B53" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C53" s="42"/>
-      <c r="D53" s="43" t="s">
+      <c r="C53"/>
+      <c r="D53" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E53" s="44" t="s">
+      <c r="E53" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54"/>
+      <c r="D54" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="B55" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D55" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="C54" s="42"/>
-      <c r="D54" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="E54" s="44" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="B55" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="44" t="s">
+      <c r="E55" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="F55" s="6">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2">
+        <v>1</v>
+      </c>
+      <c r="H55" s="2">
+        <v>1</v>
+      </c>
+      <c r="I55" s="2">
+        <v>1</v>
+      </c>
+      <c r="J55" s="2">
+        <v>1</v>
+      </c>
+      <c r="K55" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="C56"/>
+      <c r="D56" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="D55" s="45" t="s">
+      <c r="E56" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="C57"/>
+      <c r="D57" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="E55" s="46" t="s">
-        <v>107</v>
-      </c>
-      <c r="F55" s="6">
-        <v>1</v>
-      </c>
-      <c r="G55" s="2">
-        <v>1</v>
-      </c>
-      <c r="H55" s="2">
-        <v>1</v>
-      </c>
-      <c r="I55" s="2">
-        <v>1</v>
-      </c>
-      <c r="J55" s="2">
-        <v>1</v>
-      </c>
-      <c r="K55" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="C56" s="42"/>
-      <c r="D56" s="45" t="s">
+      <c r="E57" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="C58" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F58" s="6">
+        <v>1</v>
+      </c>
+      <c r="G58" s="2">
+        <v>1</v>
+      </c>
+      <c r="H58" s="2">
+        <v>1</v>
+      </c>
+      <c r="I58" s="2">
+        <v>1</v>
+      </c>
+      <c r="J58" s="2">
+        <v>1</v>
+      </c>
+      <c r="K58" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="C59"/>
+      <c r="D59" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="C60"/>
+      <c r="D60" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="24" x14ac:dyDescent="0.35">
+      <c r="C61"/>
+      <c r="D61" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="36" x14ac:dyDescent="0.35">
+      <c r="C62" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="6">
+        <v>1</v>
+      </c>
+      <c r="G62" s="2">
+        <v>1</v>
+      </c>
+      <c r="H62" s="2">
+        <v>1</v>
+      </c>
+      <c r="I62" s="2">
+        <v>1</v>
+      </c>
+      <c r="J62" s="2">
+        <v>1</v>
+      </c>
+      <c r="K62" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="48" x14ac:dyDescent="0.35">
+      <c r="C63"/>
+      <c r="D63" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="60" x14ac:dyDescent="0.35">
+      <c r="C64"/>
+      <c r="D64" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="E56" s="46" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="C57" s="42"/>
-      <c r="D57" s="45" t="s">
+      <c r="E64" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="4:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="D65" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="E57" s="44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="C58" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="D58" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="E58" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="F58" s="6">
-        <v>1</v>
-      </c>
-      <c r="G58" s="2">
-        <v>1</v>
-      </c>
-      <c r="H58" s="2">
-        <v>1</v>
-      </c>
-      <c r="I58" s="2">
-        <v>1</v>
-      </c>
-      <c r="J58" s="2">
-        <v>1</v>
-      </c>
-      <c r="K58" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="C59" s="42"/>
-      <c r="D59" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E59" s="44" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="C60" s="42"/>
-      <c r="D60" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="E60" s="44" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="24" x14ac:dyDescent="0.35">
-      <c r="C61" s="42"/>
-      <c r="D61" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="E61" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="36" x14ac:dyDescent="0.35">
-      <c r="C62" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="D62" s="43" t="s">
-        <v>56</v>
-      </c>
-      <c r="E62" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="F62" s="6">
-        <v>1</v>
-      </c>
-      <c r="G62" s="2">
-        <v>1</v>
-      </c>
-      <c r="H62" s="2">
-        <v>1</v>
-      </c>
-      <c r="I62" s="2">
-        <v>1</v>
-      </c>
-      <c r="J62" s="2">
-        <v>1</v>
-      </c>
-      <c r="K62" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="48" x14ac:dyDescent="0.35">
-      <c r="C63" s="42"/>
-      <c r="D63" s="43" t="s">
-        <v>57</v>
-      </c>
-      <c r="E63" s="44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="60" x14ac:dyDescent="0.35">
-      <c r="C64" s="42"/>
-      <c r="D64" s="45" t="s">
-        <v>185</v>
-      </c>
-      <c r="E64" s="44" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="65" spans="4:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="D65" s="45" t="s">
-        <v>186</v>
-      </c>
-      <c r="E65" s="44" t="s">
+      <c r="E65" s="4" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>